<commit_message>
added forecast for Rolling MA
</commit_message>
<xml_diff>
--- a/SystemFiles/data-processed/Compare_Forecasts_01to03.xlsx
+++ b/SystemFiles/data-processed/Compare_Forecasts_01to03.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MTech\sem1\Project\ISS_MR_2021_Product_Forecasting\SystemFiles\data-processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{613F5F43-099E-4914-8E81-0FA6758196E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8D4B47-92C5-4FFC-BB62-E0DA855153E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compare_Forecasts_01to03" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="41">
   <si>
     <t>test</t>
   </si>
@@ -129,11 +140,26 @@
   <si>
     <t>months</t>
   </si>
+  <si>
+    <t>Rolling MA</t>
+  </si>
+  <si>
+    <t>RollingMA</t>
+  </si>
+  <si>
+    <t>SARIMA / MA</t>
+  </si>
+  <si>
+    <t>LSTM/ SARIMA / MA</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -904,7 +930,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -920,25 +946,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -967,28 +992,32 @@
     <xf numFmtId="0" fontId="16" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -996,10 +1025,19 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1356,11 +1394,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U47" sqref="U47"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V66" sqref="V66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,87 +1408,107 @@
     <col min="6" max="6" width="9.88671875" customWidth="1"/>
     <col min="7" max="7" width="3.5546875" style="6" customWidth="1"/>
     <col min="11" max="11" width="9.88671875" customWidth="1"/>
-    <col min="12" max="12" width="2.5546875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="3.33203125" customWidth="1"/>
     <col min="16" max="16" width="9.88671875" customWidth="1"/>
+    <col min="17" max="17" width="2.5546875" style="6" customWidth="1"/>
+    <col min="21" max="21" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="24"/>
-      <c r="B1" s="25"/>
-      <c r="C1" s="15" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
-      <c r="H1" s="18" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="H1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="20"/>
-      <c r="M1" s="21" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="25"/>
+      <c r="M1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="25"/>
+      <c r="R1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="13" t="s">
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="35" t="s">
+      <c r="C2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="19" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="35" t="s">
+      <c r="H2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="35" t="s">
+      <c r="M2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="36" t="s">
+      <c r="P2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="14"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q2" s="3"/>
+      <c r="R2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" s="30"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="5">
@@ -1463,7 +1521,7 @@
         <f>D3-C3</f>
         <v>-2</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="34">
         <f>SUM(E3:E5)</f>
         <v>-9</v>
       </c>
@@ -1477,7 +1535,7 @@
         <f>I3-H3</f>
         <v>2</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="34">
         <f>SUM(J3:J5)</f>
         <v>3</v>
       </c>
@@ -1485,25 +1543,39 @@
         <v>2</v>
       </c>
       <c r="N3" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O3" s="6">
         <f>N3-M3</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="37">
+        <v>1</v>
+      </c>
+      <c r="P3" s="38">
         <f>SUM(O3:O5)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="5">
+        <v>2</v>
+      </c>
+      <c r="S3" s="6">
+        <v>2</v>
+      </c>
+      <c r="T3" s="6">
+        <f>S3-R3</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="41">
+        <f>SUM(T3:T5)</f>
         <v>-2</v>
       </c>
-      <c r="Q3" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="V3" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="5">
@@ -1516,7 +1588,7 @@
         <f t="shared" ref="E4:E62" si="0">D4-C4</f>
         <v>-2</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="34"/>
       <c r="H4" s="5">
         <v>2</v>
       </c>
@@ -1527,120 +1599,156 @@
         <f t="shared" ref="J4:J62" si="1">I4-H4</f>
         <v>2</v>
       </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="34"/>
       <c r="M4" s="5">
         <v>2</v>
       </c>
       <c r="N4" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O4" s="6">
         <f t="shared" ref="O4:O62" si="2">N4-M4</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="11"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="38"/>
+      <c r="R4" s="5">
+        <v>2</v>
+      </c>
+      <c r="S4" s="6">
+        <v>2</v>
+      </c>
+      <c r="T4" s="6">
+        <f t="shared" ref="T4:T62" si="3">S4-R4</f>
+        <v>0</v>
+      </c>
+      <c r="U4" s="41"/>
+      <c r="V4" s="31"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="13">
         <v>5</v>
       </c>
-      <c r="D5" s="29">
-        <v>0</v>
-      </c>
-      <c r="E5" s="29">
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="H5" s="28">
+      <c r="F5" s="35"/>
+      <c r="H5" s="13">
         <v>5</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="14">
         <v>4</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="14">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="K5" s="30"/>
-      <c r="M5" s="28">
+      <c r="K5" s="35"/>
+      <c r="M5" s="13">
         <v>5</v>
       </c>
-      <c r="N5" s="29">
-        <v>3</v>
-      </c>
-      <c r="O5" s="29">
+      <c r="N5" s="14">
+        <v>3</v>
+      </c>
+      <c r="O5" s="14">
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="11"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P5" s="39"/>
+      <c r="R5" s="13">
+        <v>5</v>
+      </c>
+      <c r="S5" s="14">
+        <v>3</v>
+      </c>
+      <c r="T5" s="14">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="U5" s="42"/>
+      <c r="V5" s="31"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="31">
-        <v>1</v>
-      </c>
-      <c r="D6" s="32">
-        <v>0</v>
-      </c>
-      <c r="E6" s="32">
+      <c r="B6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F6" s="39">
-        <f t="shared" ref="F6" si="3">SUM(E6:E8)</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="31">
-        <v>1</v>
-      </c>
-      <c r="I6" s="32">
-        <v>2</v>
-      </c>
-      <c r="J6" s="32">
+      <c r="F6" s="37">
+        <f t="shared" ref="F6" si="4">SUM(E6:E8)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="15">
+        <v>1</v>
+      </c>
+      <c r="I6" s="16">
+        <v>2</v>
+      </c>
+      <c r="J6" s="16">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K6" s="33">
-        <f t="shared" ref="K6" si="4">SUM(J6:J8)</f>
-        <v>3</v>
-      </c>
-      <c r="M6" s="31">
-        <v>1</v>
-      </c>
-      <c r="N6" s="32">
-        <v>1</v>
-      </c>
-      <c r="O6" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="39">
-        <f t="shared" ref="P6" si="5">SUM(O6:O8)</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="11" t="s">
+        <f t="shared" ref="K6" si="5">SUM(J6:J8)</f>
+        <v>3</v>
+      </c>
+      <c r="M6" s="15">
+        <v>1</v>
+      </c>
+      <c r="N6" s="16">
+        <v>3</v>
+      </c>
+      <c r="O6" s="16">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P6" s="43">
+        <f t="shared" ref="P6" si="6">SUM(O6:O8)</f>
+        <v>6</v>
+      </c>
+      <c r="R6" s="15">
+        <v>1</v>
+      </c>
+      <c r="S6" s="16">
+        <v>1</v>
+      </c>
+      <c r="T6" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="37">
+        <f t="shared" ref="U6" si="7">SUM(T6:T8)</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="5">
@@ -1653,7 +1761,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F7" s="37"/>
+      <c r="F7" s="38"/>
       <c r="H7" s="5">
         <v>1</v>
       </c>
@@ -1664,120 +1772,156 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K7" s="7"/>
+      <c r="K7" s="34"/>
       <c r="M7" s="5">
         <v>1</v>
       </c>
       <c r="N7" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O7" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="11"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="P7" s="41"/>
+      <c r="R7" s="5">
+        <v>1</v>
+      </c>
+      <c r="S7" s="6">
+        <v>1</v>
+      </c>
+      <c r="T7" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U7" s="38"/>
+      <c r="V7" s="31"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="28">
-        <v>1</v>
-      </c>
-      <c r="D8" s="29">
-        <v>0</v>
-      </c>
-      <c r="E8" s="29">
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="H8" s="28">
-        <v>1</v>
-      </c>
-      <c r="I8" s="29">
-        <v>2</v>
-      </c>
-      <c r="J8" s="29">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K8" s="30"/>
-      <c r="M8" s="28">
-        <v>1</v>
-      </c>
-      <c r="N8" s="29">
-        <v>1</v>
-      </c>
-      <c r="O8" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="11"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F8" s="39"/>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="14">
+        <v>2</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="35"/>
+      <c r="M8" s="13">
+        <v>1</v>
+      </c>
+      <c r="N8" s="14">
+        <v>3</v>
+      </c>
+      <c r="O8" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P8" s="42"/>
+      <c r="R8" s="13">
+        <v>1</v>
+      </c>
+      <c r="S8" s="14">
+        <v>1</v>
+      </c>
+      <c r="T8" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="39"/>
+      <c r="V8" s="31"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="31">
+      <c r="B9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="15">
         <v>5</v>
       </c>
-      <c r="D9" s="32">
-        <v>0</v>
-      </c>
-      <c r="E9" s="32">
+      <c r="D9" s="16">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
       <c r="F9" s="33">
-        <f t="shared" ref="F9" si="6">SUM(E9:E11)</f>
+        <f t="shared" ref="F9" si="8">SUM(E9:E11)</f>
         <v>-10</v>
       </c>
-      <c r="H9" s="31">
+      <c r="H9" s="15">
         <v>5</v>
       </c>
-      <c r="I9" s="32">
-        <v>3</v>
-      </c>
-      <c r="J9" s="32">
+      <c r="I9" s="16">
+        <v>3</v>
+      </c>
+      <c r="J9" s="16">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="K9" s="33">
-        <f t="shared" ref="K9" si="7">SUM(J9:J11)</f>
+        <f t="shared" ref="K9" si="9">SUM(J9:J11)</f>
         <v>-5</v>
       </c>
-      <c r="M9" s="31">
+      <c r="M9" s="15">
         <v>5</v>
       </c>
-      <c r="N9" s="32">
+      <c r="N9" s="16">
+        <v>4</v>
+      </c>
+      <c r="O9" s="16">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="P9" s="43">
+        <f t="shared" ref="P9" si="10">SUM(O9:O11)</f>
+        <v>-2</v>
+      </c>
+      <c r="R9" s="15">
         <v>5</v>
       </c>
-      <c r="O9" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="39">
-        <f t="shared" ref="P9" si="8">SUM(O9:O11)</f>
+      <c r="S9" s="16">
+        <v>5</v>
+      </c>
+      <c r="T9" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U9" s="37">
+        <f t="shared" ref="U9" si="11">SUM(T9:T11)</f>
         <v>-1</v>
       </c>
-      <c r="Q9" s="11" t="s">
+      <c r="V9" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="5">
@@ -1790,7 +1934,7 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="34"/>
       <c r="H10" s="5">
         <v>4</v>
       </c>
@@ -1801,7 +1945,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="K10" s="7"/>
+      <c r="K10" s="34"/>
       <c r="M10" s="5">
         <v>4</v>
       </c>
@@ -1812,56 +1956,78 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="11"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P10" s="41"/>
+      <c r="R10" s="5">
+        <v>4</v>
+      </c>
+      <c r="S10" s="6">
+        <v>4</v>
+      </c>
+      <c r="T10" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U10" s="38"/>
+      <c r="V10" s="31"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="13">
         <v>5</v>
       </c>
-      <c r="D11" s="29">
-        <v>1</v>
-      </c>
-      <c r="E11" s="29">
+      <c r="D11" s="14">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14">
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="H11" s="28">
+      <c r="F11" s="35"/>
+      <c r="H11" s="13">
         <v>5</v>
       </c>
-      <c r="I11" s="29">
-        <v>3</v>
-      </c>
-      <c r="J11" s="29">
+      <c r="I11" s="14">
+        <v>3</v>
+      </c>
+      <c r="J11" s="14">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="K11" s="30"/>
-      <c r="M11" s="28">
+      <c r="K11" s="35"/>
+      <c r="M11" s="13">
         <v>5</v>
       </c>
-      <c r="N11" s="29">
+      <c r="N11" s="14">
         <v>4</v>
       </c>
-      <c r="O11" s="29">
+      <c r="O11" s="14">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="11"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P11" s="42"/>
+      <c r="R11" s="13">
+        <v>5</v>
+      </c>
+      <c r="S11" s="14">
+        <v>4</v>
+      </c>
+      <c r="T11" s="14">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="U11" s="39"/>
+      <c r="V11" s="31"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="5">
@@ -1874,8 +2040,8 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F12" s="7">
-        <f t="shared" ref="F12" si="9">SUM(E12:E14)</f>
+      <c r="F12" s="34">
+        <f t="shared" ref="F12" si="12">SUM(E12:E14)</f>
         <v>1</v>
       </c>
       <c r="H12" s="5">
@@ -1888,33 +2054,47 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K12" s="7">
-        <f t="shared" ref="K12" si="10">SUM(J12:J14)</f>
+      <c r="K12" s="34">
+        <f t="shared" ref="K12" si="13">SUM(J12:J14)</f>
         <v>5</v>
       </c>
       <c r="M12" s="5">
         <v>0</v>
       </c>
       <c r="N12" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O12" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="37">
-        <f t="shared" ref="P12" si="11">SUM(O12:O14)</f>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="41">
+        <f t="shared" ref="P12" si="14">SUM(O12:O14)</f>
+        <v>8</v>
+      </c>
+      <c r="R12" s="5">
+        <v>0</v>
+      </c>
+      <c r="S12" s="6">
+        <v>0</v>
+      </c>
+      <c r="T12" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U12" s="38">
+        <f t="shared" ref="U12" si="15">SUM(T12:T14)</f>
+        <v>0</v>
+      </c>
+      <c r="V12" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="5">
@@ -1927,7 +2107,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="34"/>
       <c r="H13" s="5">
         <v>0</v>
       </c>
@@ -1938,25 +2118,36 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K13" s="7"/>
+      <c r="K13" s="34"/>
       <c r="M13" s="5">
         <v>0</v>
       </c>
       <c r="N13" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O13" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="11"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="P13" s="41"/>
+      <c r="R13" s="5">
+        <v>0</v>
+      </c>
+      <c r="S13" s="6">
+        <v>0</v>
+      </c>
+      <c r="T13" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U13" s="38"/>
+      <c r="V13" s="31"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="5">
@@ -1969,7 +2160,7 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="34"/>
       <c r="H14" s="5">
         <v>1</v>
       </c>
@@ -1980,78 +2171,103 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K14" s="7"/>
+      <c r="K14" s="34"/>
       <c r="M14" s="5">
         <v>1</v>
       </c>
       <c r="N14" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O14" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="11"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="P14" s="41"/>
+      <c r="R14" s="5">
+        <v>1</v>
+      </c>
+      <c r="S14" s="6">
+        <v>1</v>
+      </c>
+      <c r="T14" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U14" s="38"/>
+      <c r="V14" s="31"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="31">
-        <v>3</v>
-      </c>
-      <c r="D15" s="32">
+      <c r="B15" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="15">
+        <v>3</v>
+      </c>
+      <c r="D15" s="16">
         <v>4</v>
       </c>
-      <c r="E15" s="32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F15" s="39">
-        <f t="shared" ref="F15" si="12">SUM(E15:E17)</f>
-        <v>2</v>
-      </c>
-      <c r="H15" s="31">
-        <v>3</v>
-      </c>
-      <c r="I15" s="32">
-        <v>2</v>
-      </c>
-      <c r="J15" s="32">
+      <c r="E15" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="37">
+        <f t="shared" ref="F15" si="16">SUM(E15:E17)</f>
+        <v>2</v>
+      </c>
+      <c r="H15" s="15">
+        <v>3</v>
+      </c>
+      <c r="I15" s="16">
+        <v>2</v>
+      </c>
+      <c r="J15" s="16">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="K15" s="39">
-        <f t="shared" ref="K15" si="13">SUM(J15:J17)</f>
-        <v>2</v>
-      </c>
-      <c r="M15" s="31">
-        <v>3</v>
-      </c>
-      <c r="N15" s="32">
-        <v>3</v>
-      </c>
-      <c r="O15" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="39">
-        <f t="shared" ref="P15" si="14">SUM(O15:O17)</f>
-        <v>2</v>
-      </c>
-      <c r="Q15" s="11" t="s">
+      <c r="K15" s="37">
+        <f t="shared" ref="K15" si="17">SUM(J15:J17)</f>
+        <v>2</v>
+      </c>
+      <c r="M15" s="15">
+        <v>3</v>
+      </c>
+      <c r="N15" s="16">
+        <v>2</v>
+      </c>
+      <c r="O15" s="16">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="P15" s="37">
+        <f t="shared" ref="P15" si="18">SUM(O15:O17)</f>
+        <v>2</v>
+      </c>
+      <c r="R15" s="15">
+        <v>3</v>
+      </c>
+      <c r="S15" s="16">
+        <v>3</v>
+      </c>
+      <c r="T15" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="37">
+        <f t="shared" ref="U15" si="19">SUM(T15:T17)</f>
+        <v>2</v>
+      </c>
+      <c r="V15" s="31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="5">
@@ -2064,7 +2280,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F16" s="37"/>
+      <c r="F16" s="38"/>
       <c r="H16" s="5">
         <v>1</v>
       </c>
@@ -2075,7 +2291,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K16" s="37"/>
+      <c r="K16" s="38"/>
       <c r="M16" s="5">
         <v>1</v>
       </c>
@@ -2086,56 +2302,78 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="11"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P16" s="38"/>
+      <c r="R16" s="5">
+        <v>1</v>
+      </c>
+      <c r="S16" s="6">
+        <v>2</v>
+      </c>
+      <c r="T16" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U16" s="38"/>
+      <c r="V16" s="31"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="28">
-        <v>0</v>
-      </c>
-      <c r="D17" s="29">
-        <v>0</v>
-      </c>
-      <c r="E17" s="29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="38"/>
-      <c r="H17" s="28">
-        <v>0</v>
-      </c>
-      <c r="I17" s="29">
-        <v>2</v>
-      </c>
-      <c r="J17" s="29">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="K17" s="38"/>
-      <c r="M17" s="28">
-        <v>0</v>
-      </c>
-      <c r="N17" s="29">
-        <v>1</v>
-      </c>
-      <c r="O17" s="29">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="11"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C17" s="13">
+        <v>0</v>
+      </c>
+      <c r="D17" s="14">
+        <v>0</v>
+      </c>
+      <c r="E17" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="39"/>
+      <c r="H17" s="13">
+        <v>0</v>
+      </c>
+      <c r="I17" s="14">
+        <v>2</v>
+      </c>
+      <c r="J17" s="14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K17" s="39"/>
+      <c r="M17" s="13">
+        <v>0</v>
+      </c>
+      <c r="N17" s="14">
+        <v>2</v>
+      </c>
+      <c r="O17" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P17" s="39"/>
+      <c r="R17" s="13">
+        <v>0</v>
+      </c>
+      <c r="S17" s="14">
+        <v>1</v>
+      </c>
+      <c r="T17" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U17" s="39"/>
+      <c r="V17" s="31"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="5">
@@ -2148,8 +2386,8 @@
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="F18" s="7">
-        <f t="shared" ref="F18:F30" si="15">SUM(E18:E20)</f>
+      <c r="F18" s="34">
+        <f t="shared" ref="F18:F30" si="20">SUM(E18:E20)</f>
         <v>-5</v>
       </c>
       <c r="H18" s="5">
@@ -2162,33 +2400,47 @@
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="K18" s="7">
-        <f t="shared" ref="K18:K30" si="16">SUM(J18:J20)</f>
+      <c r="K18" s="34">
+        <f t="shared" ref="K18:K30" si="21">SUM(J18:J20)</f>
         <v>-2</v>
       </c>
       <c r="M18" s="5">
         <v>3</v>
       </c>
       <c r="N18" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O18" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="37">
-        <f t="shared" ref="P18:P30" si="17">SUM(O18:O20)</f>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="11" t="s">
+        <v>-2</v>
+      </c>
+      <c r="P18" s="41">
+        <f t="shared" ref="P18" si="22">SUM(O18:O20)</f>
+        <v>-2</v>
+      </c>
+      <c r="R18" s="5">
+        <v>3</v>
+      </c>
+      <c r="S18" s="6">
+        <v>3</v>
+      </c>
+      <c r="T18" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U18" s="38">
+        <f t="shared" ref="U18:U30" si="23">SUM(T18:T20)</f>
+        <v>0</v>
+      </c>
+      <c r="V18" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="5">
@@ -2201,7 +2453,7 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="34"/>
       <c r="H19" s="5">
         <v>1</v>
       </c>
@@ -2212,7 +2464,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K19" s="7"/>
+      <c r="K19" s="34"/>
       <c r="M19" s="5">
         <v>1</v>
       </c>
@@ -2223,14 +2475,25 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="11"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P19" s="41"/>
+      <c r="R19" s="5">
+        <v>1</v>
+      </c>
+      <c r="S19" s="6">
+        <v>1</v>
+      </c>
+      <c r="T19" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U19" s="38"/>
+      <c r="V19" s="31"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="5">
@@ -2243,7 +2506,7 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="34"/>
       <c r="H20" s="5">
         <v>1</v>
       </c>
@@ -2254,7 +2517,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K20" s="7"/>
+      <c r="K20" s="34"/>
       <c r="M20" s="5">
         <v>1</v>
       </c>
@@ -2265,67 +2528,92 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="11"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P20" s="41"/>
+      <c r="R20" s="5">
+        <v>1</v>
+      </c>
+      <c r="S20" s="6">
+        <v>1</v>
+      </c>
+      <c r="T20" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="38"/>
+      <c r="V20" s="31"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="31">
-        <v>0</v>
-      </c>
-      <c r="D21" s="32">
-        <v>0</v>
-      </c>
-      <c r="E21" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="39">
-        <f t="shared" ref="F21:F33" si="18">SUM(E21:E23)</f>
+      <c r="B21" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="15">
+        <v>0</v>
+      </c>
+      <c r="D21" s="16">
+        <v>0</v>
+      </c>
+      <c r="E21" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="37">
+        <f t="shared" ref="F21:F33" si="24">SUM(E21:E23)</f>
         <v>-3</v>
       </c>
-      <c r="H21" s="31">
-        <v>0</v>
-      </c>
-      <c r="I21" s="32">
-        <v>2</v>
-      </c>
-      <c r="J21" s="32">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="K21" s="39">
-        <f t="shared" ref="K21:K33" si="19">SUM(J21:J23)</f>
-        <v>3</v>
-      </c>
-      <c r="M21" s="31">
-        <v>0</v>
-      </c>
-      <c r="N21" s="32">
-        <v>1</v>
-      </c>
-      <c r="O21" s="32">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P21" s="39">
-        <f t="shared" ref="P21:P33" si="20">SUM(O21:O23)</f>
-        <v>3</v>
-      </c>
-      <c r="Q21" s="11" t="s">
+      <c r="H21" s="15">
+        <v>0</v>
+      </c>
+      <c r="I21" s="16">
+        <v>2</v>
+      </c>
+      <c r="J21" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K21" s="37">
+        <f t="shared" ref="K21:K33" si="25">SUM(J21:J23)</f>
+        <v>3</v>
+      </c>
+      <c r="M21" s="15">
+        <v>0</v>
+      </c>
+      <c r="N21" s="16">
+        <v>2</v>
+      </c>
+      <c r="O21" s="16">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P21" s="37">
+        <f t="shared" ref="P21" si="26">SUM(O21:O23)</f>
+        <v>3</v>
+      </c>
+      <c r="R21" s="15">
+        <v>0</v>
+      </c>
+      <c r="S21" s="16">
+        <v>1</v>
+      </c>
+      <c r="T21" s="16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U21" s="37">
+        <f t="shared" ref="U21:U33" si="27">SUM(T21:T23)</f>
+        <v>3</v>
+      </c>
+      <c r="V21" s="31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="5">
@@ -2338,7 +2626,7 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="38"/>
       <c r="H22" s="5">
         <v>2</v>
       </c>
@@ -2349,7 +2637,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K22" s="37"/>
+      <c r="K22" s="38"/>
       <c r="M22" s="5">
         <v>2</v>
       </c>
@@ -2360,56 +2648,78 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="11"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P22" s="38"/>
+      <c r="R22" s="5">
+        <v>2</v>
+      </c>
+      <c r="S22" s="6">
+        <v>2</v>
+      </c>
+      <c r="T22" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U22" s="38"/>
+      <c r="V22" s="31"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="28">
-        <v>1</v>
-      </c>
-      <c r="D23" s="29">
-        <v>0</v>
-      </c>
-      <c r="E23" s="29">
+      <c r="C23" s="13">
+        <v>1</v>
+      </c>
+      <c r="D23" s="14">
+        <v>0</v>
+      </c>
+      <c r="E23" s="14">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="H23" s="28">
-        <v>1</v>
-      </c>
-      <c r="I23" s="29">
-        <v>2</v>
-      </c>
-      <c r="J23" s="29">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K23" s="38"/>
-      <c r="M23" s="28">
-        <v>1</v>
-      </c>
-      <c r="N23" s="29">
-        <v>3</v>
-      </c>
-      <c r="O23" s="29">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="11"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F23" s="39"/>
+      <c r="H23" s="13">
+        <v>1</v>
+      </c>
+      <c r="I23" s="14">
+        <v>2</v>
+      </c>
+      <c r="J23" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K23" s="39"/>
+      <c r="M23" s="13">
+        <v>1</v>
+      </c>
+      <c r="N23" s="14">
+        <v>2</v>
+      </c>
+      <c r="O23" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P23" s="39"/>
+      <c r="R23" s="13">
+        <v>1</v>
+      </c>
+      <c r="S23" s="14">
+        <v>3</v>
+      </c>
+      <c r="T23" s="14">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U23" s="39"/>
+      <c r="V23" s="31"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="5">
@@ -2422,8 +2732,8 @@
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="F24" s="7">
-        <f t="shared" ref="F24" si="21">SUM(E24:E26)</f>
+      <c r="F24" s="34">
+        <f t="shared" ref="F24" si="28">SUM(E24:E26)</f>
         <v>-4</v>
       </c>
       <c r="H24" s="5">
@@ -2436,33 +2746,47 @@
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="K24" s="7">
-        <f t="shared" ref="K24" si="22">SUM(J24:J26)</f>
+      <c r="K24" s="34">
+        <f t="shared" ref="K24" si="29">SUM(J24:J26)</f>
         <v>-2</v>
       </c>
       <c r="M24" s="5">
         <v>3</v>
       </c>
       <c r="N24" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O24" s="6">
         <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="P24" s="41">
+        <f t="shared" ref="P24" si="30">SUM(O24:O26)</f>
+        <v>-5</v>
+      </c>
+      <c r="R24" s="5">
+        <v>3</v>
+      </c>
+      <c r="S24" s="6">
+        <v>2</v>
+      </c>
+      <c r="T24" s="6">
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="P24" s="37">
-        <f t="shared" ref="P24" si="23">SUM(O24:O26)</f>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="11" t="s">
+      <c r="U24" s="38">
+        <f t="shared" ref="U24" si="31">SUM(T24:T26)</f>
+        <v>0</v>
+      </c>
+      <c r="V24" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="5">
@@ -2475,7 +2799,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="34"/>
       <c r="H25" s="5">
         <v>1</v>
       </c>
@@ -2486,25 +2810,36 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K25" s="7"/>
+      <c r="K25" s="34"/>
       <c r="M25" s="5">
         <v>1</v>
       </c>
       <c r="N25" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="11"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-1</v>
+      </c>
+      <c r="P25" s="41"/>
+      <c r="R25" s="5">
+        <v>1</v>
+      </c>
+      <c r="S25" s="6">
+        <v>1</v>
+      </c>
+      <c r="T25" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U25" s="38"/>
+      <c r="V25" s="31"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="5">
@@ -2517,7 +2852,7 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="34"/>
       <c r="H26" s="5">
         <v>1</v>
       </c>
@@ -2528,78 +2863,103 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K26" s="7"/>
+      <c r="K26" s="34"/>
       <c r="M26" s="5">
         <v>1</v>
       </c>
       <c r="N26" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O26" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P26" s="37"/>
-      <c r="Q26" s="11"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-1</v>
+      </c>
+      <c r="P26" s="41"/>
+      <c r="R26" s="5">
+        <v>1</v>
+      </c>
+      <c r="S26" s="6">
+        <v>2</v>
+      </c>
+      <c r="T26" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U26" s="38"/>
+      <c r="V26" s="31"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="31">
-        <v>2</v>
-      </c>
-      <c r="D27" s="32">
-        <v>0</v>
-      </c>
-      <c r="E27" s="32">
+      <c r="B27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="15">
+        <v>2</v>
+      </c>
+      <c r="D27" s="16">
+        <v>0</v>
+      </c>
+      <c r="E27" s="16">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="F27" s="33">
-        <f t="shared" ref="F27" si="24">SUM(E27:E29)</f>
+        <f t="shared" ref="F27" si="32">SUM(E27:E29)</f>
         <v>-5</v>
       </c>
-      <c r="H27" s="31">
-        <v>2</v>
-      </c>
-      <c r="I27" s="32">
-        <v>2</v>
-      </c>
-      <c r="J27" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="39">
-        <f t="shared" ref="K27" si="25">SUM(J27:J29)</f>
-        <v>1</v>
-      </c>
-      <c r="M27" s="31">
-        <v>2</v>
-      </c>
-      <c r="N27" s="32">
-        <v>2</v>
-      </c>
-      <c r="O27" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="39">
-        <f t="shared" ref="P27" si="26">SUM(O27:O29)</f>
-        <v>1</v>
-      </c>
-      <c r="Q27" s="11" t="s">
+      <c r="H27" s="15">
+        <v>2</v>
+      </c>
+      <c r="I27" s="16">
+        <v>2</v>
+      </c>
+      <c r="J27" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="37">
+        <f t="shared" ref="K27" si="33">SUM(J27:J29)</f>
+        <v>1</v>
+      </c>
+      <c r="M27" s="15">
+        <v>2</v>
+      </c>
+      <c r="N27" s="16">
+        <v>0</v>
+      </c>
+      <c r="O27" s="16">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="P27" s="43">
+        <f t="shared" ref="P27" si="34">SUM(O27:O29)</f>
+        <v>-5</v>
+      </c>
+      <c r="R27" s="15">
+        <v>2</v>
+      </c>
+      <c r="S27" s="16">
+        <v>2</v>
+      </c>
+      <c r="T27" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U27" s="37">
+        <f t="shared" ref="U27" si="35">SUM(T27:T29)</f>
+        <v>1</v>
+      </c>
+      <c r="V27" s="31" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="5">
@@ -2612,7 +2972,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="34"/>
       <c r="H28" s="5">
         <v>0</v>
       </c>
@@ -2623,67 +2983,89 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K28" s="37"/>
+      <c r="K28" s="38"/>
       <c r="M28" s="5">
         <v>0</v>
       </c>
       <c r="N28" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O28" s="6">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="11"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="P28" s="41"/>
+      <c r="R28" s="5">
+        <v>0</v>
+      </c>
+      <c r="S28" s="6">
+        <v>2</v>
+      </c>
+      <c r="T28" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U28" s="38"/>
+      <c r="V28" s="31"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="28">
-        <v>3</v>
-      </c>
-      <c r="D29" s="29">
-        <v>0</v>
-      </c>
-      <c r="E29" s="29">
+      <c r="C29" s="13">
+        <v>3</v>
+      </c>
+      <c r="D29" s="14">
+        <v>0</v>
+      </c>
+      <c r="E29" s="14">
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="F29" s="30"/>
-      <c r="H29" s="28">
-        <v>3</v>
-      </c>
-      <c r="I29" s="29">
-        <v>2</v>
-      </c>
-      <c r="J29" s="29">
+      <c r="F29" s="35"/>
+      <c r="H29" s="13">
+        <v>3</v>
+      </c>
+      <c r="I29" s="14">
+        <v>2</v>
+      </c>
+      <c r="J29" s="14">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="K29" s="38"/>
-      <c r="M29" s="28">
-        <v>3</v>
-      </c>
-      <c r="N29" s="29">
-        <v>2</v>
-      </c>
-      <c r="O29" s="29">
-        <f t="shared" si="2"/>
+      <c r="K29" s="39"/>
+      <c r="M29" s="13">
+        <v>3</v>
+      </c>
+      <c r="N29" s="14">
+        <v>0</v>
+      </c>
+      <c r="O29" s="14">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="P29" s="42"/>
+      <c r="R29" s="13">
+        <v>3</v>
+      </c>
+      <c r="S29" s="14">
+        <v>2</v>
+      </c>
+      <c r="T29" s="14">
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="P29" s="38"/>
-      <c r="Q29" s="11"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="U29" s="39"/>
+      <c r="V29" s="31"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="5">
@@ -2696,8 +3078,8 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F30" s="7">
-        <f t="shared" si="15"/>
+      <c r="F30" s="34">
+        <f t="shared" si="20"/>
         <v>8</v>
       </c>
       <c r="H30" s="5">
@@ -2710,33 +3092,47 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K30" s="37">
-        <f t="shared" si="16"/>
+      <c r="K30" s="38">
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="M30" s="5">
         <v>0</v>
       </c>
       <c r="N30" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="7">
-        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="P30" s="38">
+        <f t="shared" ref="P30" si="36">SUM(O30:O32)</f>
+        <v>0</v>
+      </c>
+      <c r="R30" s="5">
+        <v>0</v>
+      </c>
+      <c r="S30" s="6">
+        <v>0</v>
+      </c>
+      <c r="T30" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U30" s="34">
+        <f t="shared" si="23"/>
         <v>-2</v>
       </c>
-      <c r="Q30" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="V30" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="5">
@@ -2749,7 +3145,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="34"/>
       <c r="H31" s="5">
         <v>3</v>
       </c>
@@ -2760,7 +3156,7 @@
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="K31" s="37"/>
+      <c r="K31" s="38"/>
       <c r="M31" s="5">
         <v>3</v>
       </c>
@@ -2771,14 +3167,25 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="11"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P31" s="38"/>
+      <c r="R31" s="5">
+        <v>3</v>
+      </c>
+      <c r="S31" s="6">
+        <v>1</v>
+      </c>
+      <c r="T31" s="6">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="U31" s="34"/>
+      <c r="V31" s="31"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="5">
@@ -2791,7 +3198,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F32" s="7"/>
+      <c r="F32" s="34"/>
       <c r="H32" s="5">
         <v>0</v>
       </c>
@@ -2802,78 +3209,103 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K32" s="37"/>
+      <c r="K32" s="38"/>
       <c r="M32" s="5">
         <v>0</v>
       </c>
       <c r="N32" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="11"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P32" s="38"/>
+      <c r="R32" s="5">
+        <v>0</v>
+      </c>
+      <c r="S32" s="6">
+        <v>0</v>
+      </c>
+      <c r="T32" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U32" s="34"/>
+      <c r="V32" s="31"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="31">
-        <v>1</v>
-      </c>
-      <c r="D33" s="32">
-        <v>0</v>
-      </c>
-      <c r="E33" s="32">
+      <c r="B33" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="15">
+        <v>1</v>
+      </c>
+      <c r="D33" s="16">
+        <v>0</v>
+      </c>
+      <c r="E33" s="16">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="F33" s="33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>-2</v>
       </c>
-      <c r="H33" s="31">
-        <v>1</v>
-      </c>
-      <c r="I33" s="32">
-        <v>1</v>
-      </c>
-      <c r="J33" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="39">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="31">
-        <v>1</v>
-      </c>
-      <c r="N33" s="32">
-        <v>1</v>
-      </c>
-      <c r="O33" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P33" s="39">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="Q33" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H33" s="15">
+        <v>1</v>
+      </c>
+      <c r="I33" s="16">
+        <v>1</v>
+      </c>
+      <c r="J33" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="37">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="15">
+        <v>1</v>
+      </c>
+      <c r="N33" s="16">
+        <v>1</v>
+      </c>
+      <c r="O33" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P33" s="37">
+        <f t="shared" ref="P33" si="37">SUM(O33:O35)</f>
+        <v>0</v>
+      </c>
+      <c r="R33" s="15">
+        <v>1</v>
+      </c>
+      <c r="S33" s="16">
+        <v>1</v>
+      </c>
+      <c r="T33" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U33" s="37">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="V33" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="5">
@@ -2886,7 +3318,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F34" s="7"/>
+      <c r="F34" s="34"/>
       <c r="H34" s="5">
         <v>1</v>
       </c>
@@ -2897,7 +3329,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K34" s="37"/>
+      <c r="K34" s="38"/>
       <c r="M34" s="5">
         <v>1</v>
       </c>
@@ -2908,56 +3340,78 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P34" s="37"/>
-      <c r="Q34" s="11"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P34" s="38"/>
+      <c r="R34" s="5">
+        <v>1</v>
+      </c>
+      <c r="S34" s="6">
+        <v>1</v>
+      </c>
+      <c r="T34" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U34" s="38"/>
+      <c r="V34" s="31"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="28">
-        <v>1</v>
-      </c>
-      <c r="D35" s="29">
-        <v>0</v>
-      </c>
-      <c r="E35" s="29">
+      <c r="C35" s="13">
+        <v>1</v>
+      </c>
+      <c r="D35" s="14">
+        <v>0</v>
+      </c>
+      <c r="E35" s="14">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F35" s="30"/>
-      <c r="H35" s="28">
-        <v>1</v>
-      </c>
-      <c r="I35" s="29">
-        <v>1</v>
-      </c>
-      <c r="J35" s="29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K35" s="38"/>
-      <c r="M35" s="28">
-        <v>1</v>
-      </c>
-      <c r="N35" s="29">
-        <v>1</v>
-      </c>
-      <c r="O35" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P35" s="38"/>
-      <c r="Q35" s="11"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F35" s="35"/>
+      <c r="H35" s="13">
+        <v>1</v>
+      </c>
+      <c r="I35" s="14">
+        <v>1</v>
+      </c>
+      <c r="J35" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="39"/>
+      <c r="M35" s="13">
+        <v>1</v>
+      </c>
+      <c r="N35" s="14">
+        <v>1</v>
+      </c>
+      <c r="O35" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="39"/>
+      <c r="R35" s="13">
+        <v>1</v>
+      </c>
+      <c r="S35" s="14">
+        <v>1</v>
+      </c>
+      <c r="T35" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U35" s="39"/>
+      <c r="V35" s="31"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="5">
@@ -2970,7 +3424,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F36" s="37">
+      <c r="F36" s="41">
         <f>SUM(E36:E38)</f>
         <v>2</v>
       </c>
@@ -2984,7 +3438,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K36" s="37">
+      <c r="K36" s="41">
         <f>SUM(J36:J38)</f>
         <v>2</v>
       </c>
@@ -2998,19 +3452,33 @@
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="P36" s="37">
+      <c r="P36" s="38">
         <f>SUM(O36:O38)</f>
+        <v>-1</v>
+      </c>
+      <c r="R36" s="5">
+        <v>2</v>
+      </c>
+      <c r="S36" s="6">
+        <v>1</v>
+      </c>
+      <c r="T36" s="6">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="U36" s="41">
+        <f>SUM(T36:T38)</f>
         <v>-2</v>
       </c>
-      <c r="Q36" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="V36" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="5">
@@ -3023,7 +3491,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F37" s="37"/>
+      <c r="F37" s="41"/>
       <c r="H37" s="5">
         <v>0</v>
       </c>
@@ -3034,25 +3502,36 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="K37" s="37"/>
+      <c r="K37" s="41"/>
       <c r="M37" s="5">
         <v>0</v>
       </c>
       <c r="N37" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O37" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P37" s="37"/>
-      <c r="Q37" s="11"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P37" s="38"/>
+      <c r="R37" s="5">
+        <v>0</v>
+      </c>
+      <c r="S37" s="6">
+        <v>0</v>
+      </c>
+      <c r="T37" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U37" s="41"/>
+      <c r="V37" s="31"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="5">
@@ -3065,7 +3544,7 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F38" s="37"/>
+      <c r="F38" s="41"/>
       <c r="H38" s="5">
         <v>2</v>
       </c>
@@ -3076,7 +3555,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K38" s="37"/>
+      <c r="K38" s="41"/>
       <c r="M38" s="5">
         <v>2</v>
       </c>
@@ -3087,67 +3566,92 @@
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="P38" s="37"/>
-      <c r="Q38" s="11"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P38" s="38"/>
+      <c r="R38" s="5">
+        <v>2</v>
+      </c>
+      <c r="S38" s="6">
+        <v>1</v>
+      </c>
+      <c r="T38" s="6">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="U38" s="41"/>
+      <c r="V38" s="31"/>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="31">
+      <c r="B39" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="15">
         <v>4</v>
       </c>
-      <c r="D39" s="32">
-        <v>0</v>
-      </c>
-      <c r="E39" s="32">
+      <c r="D39" s="16">
+        <v>0</v>
+      </c>
+      <c r="E39" s="16">
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
       <c r="F39" s="33">
-        <f t="shared" ref="F39" si="27">SUM(E39:E41)</f>
+        <f t="shared" ref="F39" si="38">SUM(E39:E41)</f>
         <v>-9</v>
       </c>
-      <c r="H39" s="31">
+      <c r="H39" s="15">
         <v>4</v>
       </c>
-      <c r="I39" s="32">
-        <v>2</v>
-      </c>
-      <c r="J39" s="32">
+      <c r="I39" s="16">
+        <v>2</v>
+      </c>
+      <c r="J39" s="16">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="K39" s="33">
-        <f t="shared" ref="K39" si="28">SUM(J39:J41)</f>
+        <f t="shared" ref="K39" si="39">SUM(J39:J41)</f>
         <v>-3</v>
       </c>
-      <c r="M39" s="31">
+      <c r="M39" s="15">
         <v>4</v>
       </c>
-      <c r="N39" s="32">
+      <c r="N39" s="16">
+        <v>1</v>
+      </c>
+      <c r="O39" s="16">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="P39" s="43">
+        <f t="shared" ref="P39" si="40">SUM(O39:O41)</f>
+        <v>-6</v>
+      </c>
+      <c r="R39" s="15">
         <v>4</v>
       </c>
-      <c r="O39" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P39" s="39">
-        <f t="shared" ref="P39" si="29">SUM(O39:O41)</f>
+      <c r="S39" s="16">
+        <v>4</v>
+      </c>
+      <c r="T39" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U39" s="37">
+        <f t="shared" ref="U39" si="41">SUM(T39:T41)</f>
         <v>-1</v>
       </c>
-      <c r="Q39" s="11" t="s">
+      <c r="V39" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="5">
@@ -3160,7 +3664,7 @@
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="F40" s="7"/>
+      <c r="F40" s="34"/>
       <c r="H40" s="5">
         <v>3</v>
       </c>
@@ -3171,67 +3675,89 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="K40" s="7"/>
+      <c r="K40" s="34"/>
       <c r="M40" s="5">
         <v>3</v>
       </c>
       <c r="N40" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O40" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P40" s="37"/>
-      <c r="Q40" s="11"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-2</v>
+      </c>
+      <c r="P40" s="41"/>
+      <c r="R40" s="5">
+        <v>3</v>
+      </c>
+      <c r="S40" s="6">
+        <v>3</v>
+      </c>
+      <c r="T40" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U40" s="38"/>
+      <c r="V40" s="31"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="28">
-        <v>2</v>
-      </c>
-      <c r="D41" s="29">
-        <v>0</v>
-      </c>
-      <c r="E41" s="29">
+      <c r="C41" s="13">
+        <v>2</v>
+      </c>
+      <c r="D41" s="14">
+        <v>0</v>
+      </c>
+      <c r="E41" s="14">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F41" s="30"/>
-      <c r="H41" s="28">
-        <v>2</v>
-      </c>
-      <c r="I41" s="29">
-        <v>2</v>
-      </c>
-      <c r="J41" s="29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K41" s="30"/>
-      <c r="M41" s="28">
-        <v>2</v>
-      </c>
-      <c r="N41" s="29">
-        <v>1</v>
-      </c>
-      <c r="O41" s="29">
+      <c r="F41" s="35"/>
+      <c r="H41" s="13">
+        <v>2</v>
+      </c>
+      <c r="I41" s="14">
+        <v>2</v>
+      </c>
+      <c r="J41" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K41" s="35"/>
+      <c r="M41" s="13">
+        <v>2</v>
+      </c>
+      <c r="N41" s="14">
+        <v>1</v>
+      </c>
+      <c r="O41" s="14">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="P41" s="38"/>
-      <c r="Q41" s="11"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P41" s="42"/>
+      <c r="R41" s="13">
+        <v>2</v>
+      </c>
+      <c r="S41" s="14">
+        <v>1</v>
+      </c>
+      <c r="T41" s="14">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="U41" s="39"/>
+      <c r="V41" s="31"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C42" s="5">
@@ -3244,8 +3770,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F42" s="7">
-        <f t="shared" ref="F42" si="30">SUM(E42:E44)</f>
+      <c r="F42" s="34">
+        <f t="shared" ref="F42" si="42">SUM(E42:E44)</f>
         <v>-2</v>
       </c>
       <c r="H42" s="5">
@@ -3258,33 +3784,47 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="K42" s="7">
-        <f t="shared" ref="K42" si="31">SUM(J42:J44)</f>
+      <c r="K42" s="34">
+        <f t="shared" ref="K42" si="43">SUM(J42:J44)</f>
         <v>-4</v>
       </c>
       <c r="M42" s="5">
         <v>1</v>
       </c>
       <c r="N42" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O42" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P42" s="37">
-        <f t="shared" ref="P42" si="32">SUM(O42:O44)</f>
-        <v>0</v>
-      </c>
-      <c r="Q42" s="11" t="s">
+        <v>-1</v>
+      </c>
+      <c r="P42" s="41">
+        <f t="shared" ref="P42" si="44">SUM(O42:O44)</f>
+        <v>-4</v>
+      </c>
+      <c r="R42" s="5">
+        <v>1</v>
+      </c>
+      <c r="S42" s="6">
+        <v>1</v>
+      </c>
+      <c r="T42" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U42" s="38">
+        <f t="shared" ref="U42" si="45">SUM(T42:T44)</f>
+        <v>0</v>
+      </c>
+      <c r="V42" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="5">
@@ -3297,7 +3837,7 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F43" s="7"/>
+      <c r="F43" s="34"/>
       <c r="H43" s="5">
         <v>1</v>
       </c>
@@ -3308,25 +3848,36 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="K43" s="7"/>
+      <c r="K43" s="34"/>
       <c r="M43" s="5">
         <v>1</v>
       </c>
       <c r="N43" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O43" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P43" s="37"/>
-      <c r="Q43" s="11"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-1</v>
+      </c>
+      <c r="P43" s="41"/>
+      <c r="R43" s="5">
+        <v>1</v>
+      </c>
+      <c r="S43" s="6">
+        <v>1</v>
+      </c>
+      <c r="T43" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U43" s="38"/>
+      <c r="V43" s="31"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="5">
@@ -3339,7 +3890,7 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F44" s="7"/>
+      <c r="F44" s="34"/>
       <c r="H44" s="5">
         <v>2</v>
       </c>
@@ -3350,78 +3901,103 @@
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="K44" s="7"/>
+      <c r="K44" s="34"/>
       <c r="M44" s="5">
         <v>2</v>
       </c>
       <c r="N44" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O44" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P44" s="37"/>
-      <c r="Q44" s="11"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-2</v>
+      </c>
+      <c r="P44" s="41"/>
+      <c r="R44" s="5">
+        <v>2</v>
+      </c>
+      <c r="S44" s="6">
+        <v>2</v>
+      </c>
+      <c r="T44" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U44" s="38"/>
+      <c r="V44" s="31"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="31">
-        <v>3</v>
-      </c>
-      <c r="D45" s="32">
+      <c r="B45" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="15">
+        <v>3</v>
+      </c>
+      <c r="D45" s="16">
         <v>5</v>
       </c>
-      <c r="E45" s="32">
+      <c r="E45" s="16">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F45" s="33">
-        <f t="shared" ref="F45" si="33">SUM(E45:E47)</f>
+        <f t="shared" ref="F45" si="46">SUM(E45:E47)</f>
         <v>9</v>
       </c>
-      <c r="H45" s="31">
-        <v>3</v>
-      </c>
-      <c r="I45" s="32">
-        <v>3</v>
-      </c>
-      <c r="J45" s="32">
+      <c r="H45" s="15">
+        <v>3</v>
+      </c>
+      <c r="I45" s="16">
+        <v>3</v>
+      </c>
+      <c r="J45" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K45" s="33">
-        <f t="shared" ref="K45" si="34">SUM(J45:J47)</f>
-        <v>3</v>
-      </c>
-      <c r="M45" s="31">
-        <v>3</v>
-      </c>
-      <c r="N45" s="32">
-        <v>2</v>
-      </c>
-      <c r="O45" s="32">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K45" si="47">SUM(J45:J47)</f>
+        <v>3</v>
+      </c>
+      <c r="M45" s="15">
+        <v>3</v>
+      </c>
+      <c r="N45" s="16">
+        <v>3</v>
+      </c>
+      <c r="O45" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P45" s="43">
+        <f t="shared" ref="P45" si="48">SUM(O45:O47)</f>
+        <v>3</v>
+      </c>
+      <c r="R45" s="15">
+        <v>3</v>
+      </c>
+      <c r="S45" s="16">
+        <v>2</v>
+      </c>
+      <c r="T45" s="16">
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="P45" s="39">
-        <f t="shared" ref="P45" si="35">SUM(O45:O47)</f>
-        <v>0</v>
-      </c>
-      <c r="Q45" s="11" t="s">
+      <c r="U45" s="37">
+        <f t="shared" ref="U45" si="49">SUM(T45:T47)</f>
+        <v>0</v>
+      </c>
+      <c r="V45" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="5">
@@ -3434,7 +4010,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="34"/>
       <c r="H46" s="5">
         <v>0</v>
       </c>
@@ -3445,67 +4021,89 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="K46" s="7"/>
+      <c r="K46" s="34"/>
       <c r="M46" s="5">
         <v>0</v>
       </c>
       <c r="N46" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O46" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P46" s="37"/>
-      <c r="Q46" s="11"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="P46" s="41"/>
+      <c r="R46" s="5">
+        <v>0</v>
+      </c>
+      <c r="S46" s="6">
+        <v>1</v>
+      </c>
+      <c r="T46" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U46" s="38"/>
+      <c r="V46" s="31"/>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="28">
-        <v>3</v>
-      </c>
-      <c r="D47" s="29">
+      <c r="C47" s="13">
+        <v>3</v>
+      </c>
+      <c r="D47" s="14">
         <v>6</v>
       </c>
-      <c r="E47" s="29">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F47" s="30"/>
-      <c r="H47" s="28">
-        <v>3</v>
-      </c>
-      <c r="I47" s="29">
-        <v>3</v>
-      </c>
-      <c r="J47" s="29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K47" s="30"/>
-      <c r="M47" s="28">
-        <v>3</v>
-      </c>
-      <c r="N47" s="29">
-        <v>3</v>
-      </c>
-      <c r="O47" s="29">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P47" s="38"/>
-      <c r="Q47" s="11"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="E47" s="14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F47" s="35"/>
+      <c r="H47" s="13">
+        <v>3</v>
+      </c>
+      <c r="I47" s="14">
+        <v>3</v>
+      </c>
+      <c r="J47" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K47" s="35"/>
+      <c r="M47" s="13">
+        <v>3</v>
+      </c>
+      <c r="N47" s="14">
+        <v>3</v>
+      </c>
+      <c r="O47" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P47" s="42"/>
+      <c r="R47" s="13">
+        <v>3</v>
+      </c>
+      <c r="S47" s="14">
+        <v>3</v>
+      </c>
+      <c r="T47" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U47" s="39"/>
+      <c r="V47" s="31"/>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="5">
@@ -3518,7 +4116,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F48" s="34">
         <f>SUM(E48:E50)</f>
         <v>8</v>
       </c>
@@ -3532,7 +4130,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K48" s="37">
+      <c r="K48" s="38">
         <f>SUM(J48:J50)</f>
         <v>1</v>
       </c>
@@ -3540,25 +4138,39 @@
         <v>2</v>
       </c>
       <c r="N48" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O48" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P48" s="7">
+        <v>2</v>
+      </c>
+      <c r="P48" s="41">
         <f>SUM(O48:O50)</f>
+        <v>4</v>
+      </c>
+      <c r="R48" s="5">
+        <v>2</v>
+      </c>
+      <c r="S48" s="6">
+        <v>2</v>
+      </c>
+      <c r="T48" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U48" s="34">
+        <f>SUM(T48:T50)</f>
         <v>-2</v>
       </c>
-      <c r="Q48" s="11" t="s">
+      <c r="V48" s="31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="5">
@@ -3571,7 +4183,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F49" s="7"/>
+      <c r="F49" s="34"/>
       <c r="H49" s="5">
         <v>3</v>
       </c>
@@ -3582,25 +4194,36 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K49" s="37"/>
+      <c r="K49" s="38"/>
       <c r="M49" s="5">
         <v>3</v>
       </c>
       <c r="N49" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O49" s="6">
         <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P49" s="41"/>
+      <c r="R49" s="5">
+        <v>3</v>
+      </c>
+      <c r="S49" s="6">
+        <v>2</v>
+      </c>
+      <c r="T49" s="6">
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="P49" s="7"/>
-      <c r="Q49" s="11"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="U49" s="34"/>
+      <c r="V49" s="31"/>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="5">
@@ -3613,7 +4236,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F50" s="7"/>
+      <c r="F50" s="34"/>
       <c r="H50" s="5">
         <v>3</v>
       </c>
@@ -3624,78 +4247,103 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K50" s="37"/>
+      <c r="K50" s="38"/>
       <c r="M50" s="5">
         <v>3</v>
       </c>
       <c r="N50" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O50" s="6">
         <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P50" s="41"/>
+      <c r="R50" s="5">
+        <v>3</v>
+      </c>
+      <c r="S50" s="6">
+        <v>2</v>
+      </c>
+      <c r="T50" s="6">
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="P50" s="7"/>
-      <c r="Q50" s="11"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="U50" s="34"/>
+      <c r="V50" s="31"/>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="31">
-        <v>0</v>
-      </c>
-      <c r="D51" s="32">
-        <v>3</v>
-      </c>
-      <c r="E51" s="32">
+      <c r="B51" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="15">
+        <v>0</v>
+      </c>
+      <c r="D51" s="16">
+        <v>3</v>
+      </c>
+      <c r="E51" s="16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F51" s="33">
-        <f t="shared" ref="F51" si="36">SUM(E51:E53)</f>
+        <f t="shared" ref="F51" si="50">SUM(E51:E53)</f>
         <v>5</v>
       </c>
-      <c r="H51" s="31">
-        <v>0</v>
-      </c>
-      <c r="I51" s="32">
-        <v>2</v>
-      </c>
-      <c r="J51" s="32">
+      <c r="H51" s="15">
+        <v>0</v>
+      </c>
+      <c r="I51" s="16">
+        <v>2</v>
+      </c>
+      <c r="J51" s="16">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K51" s="33">
-        <f t="shared" ref="K51" si="37">SUM(J51:J53)</f>
+        <f t="shared" ref="K51" si="51">SUM(J51:J53)</f>
         <v>5</v>
       </c>
-      <c r="M51" s="31">
-        <v>0</v>
-      </c>
-      <c r="N51" s="32">
-        <v>0</v>
-      </c>
-      <c r="O51" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P51" s="39">
-        <f t="shared" ref="P51" si="38">SUM(O51:O53)</f>
-        <v>1</v>
-      </c>
-      <c r="Q51" s="11" t="s">
+      <c r="M51" s="15">
+        <v>0</v>
+      </c>
+      <c r="N51" s="16">
+        <v>1</v>
+      </c>
+      <c r="O51" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P51" s="43">
+        <f t="shared" ref="P51" si="52">SUM(O51:O53)</f>
+        <v>2</v>
+      </c>
+      <c r="R51" s="15">
+        <v>0</v>
+      </c>
+      <c r="S51" s="16">
+        <v>0</v>
+      </c>
+      <c r="T51" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U51" s="37">
+        <f t="shared" ref="U51" si="53">SUM(T51:T53)</f>
+        <v>1</v>
+      </c>
+      <c r="V51" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="26" t="s">
+      <c r="B52" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C52" s="5">
@@ -3708,7 +4356,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F52" s="7"/>
+      <c r="F52" s="34"/>
       <c r="H52" s="5">
         <v>1</v>
       </c>
@@ -3719,7 +4367,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K52" s="7"/>
+      <c r="K52" s="34"/>
       <c r="M52" s="5">
         <v>1</v>
       </c>
@@ -3730,56 +4378,78 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P52" s="37"/>
-      <c r="Q52" s="11"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P52" s="41"/>
+      <c r="R52" s="5">
+        <v>1</v>
+      </c>
+      <c r="S52" s="6">
+        <v>1</v>
+      </c>
+      <c r="T52" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U52" s="38"/>
+      <c r="V52" s="31"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B53" s="26" t="s">
+      <c r="B53" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="28">
-        <v>0</v>
-      </c>
-      <c r="D53" s="29">
-        <v>2</v>
-      </c>
-      <c r="E53" s="29">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F53" s="30"/>
-      <c r="H53" s="28">
-        <v>0</v>
-      </c>
-      <c r="I53" s="29">
-        <v>2</v>
-      </c>
-      <c r="J53" s="29">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="K53" s="30"/>
-      <c r="M53" s="28">
-        <v>0</v>
-      </c>
-      <c r="N53" s="29">
-        <v>1</v>
-      </c>
-      <c r="O53" s="29">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P53" s="38"/>
-      <c r="Q53" s="11"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C53" s="13">
+        <v>0</v>
+      </c>
+      <c r="D53" s="14">
+        <v>2</v>
+      </c>
+      <c r="E53" s="14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F53" s="35"/>
+      <c r="H53" s="13">
+        <v>0</v>
+      </c>
+      <c r="I53" s="14">
+        <v>2</v>
+      </c>
+      <c r="J53" s="14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K53" s="35"/>
+      <c r="M53" s="13">
+        <v>0</v>
+      </c>
+      <c r="N53" s="14">
+        <v>1</v>
+      </c>
+      <c r="O53" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P53" s="42"/>
+      <c r="R53" s="13">
+        <v>0</v>
+      </c>
+      <c r="S53" s="14">
+        <v>1</v>
+      </c>
+      <c r="T53" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U53" s="39"/>
+      <c r="V53" s="31"/>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B54" s="26" t="s">
+      <c r="B54" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C54" s="5">
@@ -3792,8 +4462,8 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F54" s="7">
-        <f t="shared" ref="F54" si="39">SUM(E54:E56)</f>
+      <c r="F54" s="34">
+        <f t="shared" ref="F54" si="54">SUM(E54:E56)</f>
         <v>-4</v>
       </c>
       <c r="H54" s="5">
@@ -3806,33 +4476,47 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K54" s="37">
-        <f t="shared" ref="K54" si="40">SUM(J54:J56)</f>
+      <c r="K54" s="38">
+        <f t="shared" ref="K54" si="55">SUM(J54:J56)</f>
         <v>3</v>
       </c>
       <c r="M54" s="5">
         <v>2</v>
       </c>
       <c r="N54" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O54" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P54" s="37">
-        <f t="shared" ref="P54" si="41">SUM(O54:O56)</f>
-        <v>3</v>
-      </c>
-      <c r="Q54" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="P54" s="41">
+        <f t="shared" ref="P54" si="56">SUM(O54:O56)</f>
+        <v>5</v>
+      </c>
+      <c r="R54" s="5">
+        <v>2</v>
+      </c>
+      <c r="S54" s="6">
+        <v>3</v>
+      </c>
+      <c r="T54" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U54" s="38">
+        <f t="shared" ref="U54" si="57">SUM(T54:T56)</f>
+        <v>3</v>
+      </c>
+      <c r="V54" s="31" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B55" s="26" t="s">
+      <c r="B55" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="5">
@@ -3845,7 +4529,7 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F55" s="7"/>
+      <c r="F55" s="34"/>
       <c r="H55" s="5">
         <v>3</v>
       </c>
@@ -3856,25 +4540,36 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K55" s="37"/>
+      <c r="K55" s="38"/>
       <c r="M55" s="5">
         <v>3</v>
       </c>
       <c r="N55" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O55" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P55" s="37"/>
-      <c r="Q55" s="11"/>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P55" s="41"/>
+      <c r="R55" s="5">
+        <v>3</v>
+      </c>
+      <c r="S55" s="6">
+        <v>3</v>
+      </c>
+      <c r="T55" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U55" s="38"/>
+      <c r="V55" s="31"/>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B56" s="26" t="s">
+      <c r="B56" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C56" s="5">
@@ -3887,7 +4582,7 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F56" s="7"/>
+      <c r="F56" s="34"/>
       <c r="H56" s="5">
         <v>2</v>
       </c>
@@ -3898,7 +4593,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K56" s="37"/>
+      <c r="K56" s="38"/>
       <c r="M56" s="5">
         <v>2</v>
       </c>
@@ -3909,67 +4604,92 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="P56" s="37"/>
-      <c r="Q56" s="11"/>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P56" s="41"/>
+      <c r="R56" s="5">
+        <v>2</v>
+      </c>
+      <c r="S56" s="6">
+        <v>4</v>
+      </c>
+      <c r="T56" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U56" s="38"/>
+      <c r="V56" s="31"/>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B57" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" s="31">
-        <v>3</v>
-      </c>
-      <c r="D57" s="32">
-        <v>0</v>
-      </c>
-      <c r="E57" s="32">
+      <c r="B57" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="15">
+        <v>3</v>
+      </c>
+      <c r="D57" s="16">
+        <v>0</v>
+      </c>
+      <c r="E57" s="16">
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
       <c r="F57" s="33">
-        <f t="shared" ref="F57" si="42">SUM(E57:E59)</f>
+        <f t="shared" ref="F57" si="58">SUM(E57:E59)</f>
         <v>-7</v>
       </c>
-      <c r="H57" s="31">
-        <v>3</v>
-      </c>
-      <c r="I57" s="32">
-        <v>2</v>
-      </c>
-      <c r="J57" s="32">
+      <c r="H57" s="15">
+        <v>3</v>
+      </c>
+      <c r="I57" s="16">
+        <v>2</v>
+      </c>
+      <c r="J57" s="16">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="K57" s="39">
-        <f t="shared" ref="K57" si="43">SUM(J57:J59)</f>
+      <c r="K57" s="37">
+        <f t="shared" ref="K57" si="59">SUM(J57:J59)</f>
         <v>-1</v>
       </c>
-      <c r="M57" s="31">
-        <v>3</v>
-      </c>
-      <c r="N57" s="32">
-        <v>3</v>
-      </c>
-      <c r="O57" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P57" s="33">
-        <f t="shared" ref="P57" si="44">SUM(O57:O59)</f>
-        <v>3</v>
-      </c>
-      <c r="Q57" s="11" t="s">
+      <c r="M57" s="15">
+        <v>3</v>
+      </c>
+      <c r="N57" s="16">
+        <v>1</v>
+      </c>
+      <c r="O57" s="16">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="P57" s="43">
+        <f t="shared" ref="P57" si="60">SUM(O57:O59)</f>
+        <v>-4</v>
+      </c>
+      <c r="R57" s="15">
+        <v>3</v>
+      </c>
+      <c r="S57" s="16">
+        <v>3</v>
+      </c>
+      <c r="T57" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U57" s="33">
+        <f t="shared" ref="U57" si="61">SUM(T57:T59)</f>
+        <v>3</v>
+      </c>
+      <c r="V57" s="31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="26" t="s">
+      <c r="B58" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="5">
@@ -3982,7 +4702,7 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F58" s="7"/>
+      <c r="F58" s="34"/>
       <c r="H58" s="5">
         <v>2</v>
       </c>
@@ -3993,67 +4713,89 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K58" s="37"/>
+      <c r="K58" s="38"/>
       <c r="M58" s="5">
         <v>2</v>
       </c>
       <c r="N58" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O58" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="P58" s="7"/>
-      <c r="Q58" s="11"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-1</v>
+      </c>
+      <c r="P58" s="41"/>
+      <c r="R58" s="5">
+        <v>2</v>
+      </c>
+      <c r="S58" s="6">
+        <v>3</v>
+      </c>
+      <c r="T58" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U58" s="34"/>
+      <c r="V58" s="31"/>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="28">
-        <v>2</v>
-      </c>
-      <c r="D59" s="29">
-        <v>0</v>
-      </c>
-      <c r="E59" s="29">
+      <c r="C59" s="13">
+        <v>2</v>
+      </c>
+      <c r="D59" s="14">
+        <v>0</v>
+      </c>
+      <c r="E59" s="14">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F59" s="30"/>
-      <c r="H59" s="28">
-        <v>2</v>
-      </c>
-      <c r="I59" s="29">
-        <v>2</v>
-      </c>
-      <c r="J59" s="29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K59" s="38"/>
-      <c r="M59" s="28">
-        <v>2</v>
-      </c>
-      <c r="N59" s="29">
+      <c r="F59" s="35"/>
+      <c r="H59" s="13">
+        <v>2</v>
+      </c>
+      <c r="I59" s="14">
+        <v>2</v>
+      </c>
+      <c r="J59" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K59" s="39"/>
+      <c r="M59" s="13">
+        <v>2</v>
+      </c>
+      <c r="N59" s="14">
+        <v>1</v>
+      </c>
+      <c r="O59" s="14">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="P59" s="42"/>
+      <c r="R59" s="13">
+        <v>2</v>
+      </c>
+      <c r="S59" s="14">
         <v>4</v>
       </c>
-      <c r="O59" s="29">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="P59" s="30"/>
-      <c r="Q59" s="11"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T59" s="14">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U59" s="35"/>
+      <c r="V59" s="31"/>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B60" s="26" t="s">
+      <c r="B60" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C60" s="5">
@@ -4066,8 +4808,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F60" s="37">
-        <f t="shared" ref="F60" si="45">SUM(E60:E62)</f>
+      <c r="F60" s="38">
+        <f t="shared" ref="F60" si="62">SUM(E60:E62)</f>
         <v>0</v>
       </c>
       <c r="H60" s="5">
@@ -4080,33 +4822,47 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K60" s="7">
-        <f t="shared" ref="K60" si="46">SUM(J60:J62)</f>
+      <c r="K60" s="34">
+        <f t="shared" ref="K60" si="63">SUM(J60:J62)</f>
         <v>-1</v>
       </c>
       <c r="M60" s="5">
         <v>0</v>
       </c>
       <c r="N60" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O60" s="6">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="P60" s="7">
-        <f t="shared" ref="P60" si="47">SUM(O60:O62)</f>
-        <v>2</v>
-      </c>
-      <c r="Q60" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="P60" s="41">
+        <f t="shared" ref="P60" si="64">SUM(O60:O62)</f>
+        <v>-1</v>
+      </c>
+      <c r="R60" s="5">
+        <v>0</v>
+      </c>
+      <c r="S60" s="6">
+        <v>3</v>
+      </c>
+      <c r="T60" s="6">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U60" s="34">
+        <f t="shared" ref="U60" si="65">SUM(T60:T62)</f>
+        <v>2</v>
+      </c>
+      <c r="V60" s="31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C61" s="5">
@@ -4119,7 +4875,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F61" s="37"/>
+      <c r="F61" s="38"/>
       <c r="H61" s="5">
         <v>4</v>
       </c>
@@ -4130,144 +4886,151 @@
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
-      <c r="K61" s="7"/>
+      <c r="K61" s="34"/>
       <c r="M61" s="5">
         <v>4</v>
       </c>
       <c r="N61" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O61" s="6">
         <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="P61" s="41"/>
+      <c r="R61" s="5">
+        <v>4</v>
+      </c>
+      <c r="S61" s="6">
+        <v>3</v>
+      </c>
+      <c r="T61" s="6">
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="P61" s="7"/>
-      <c r="Q61" s="11"/>
-    </row>
-    <row r="62" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="8" t="s">
+      <c r="U61" s="34"/>
+      <c r="V61" s="31"/>
+    </row>
+    <row r="62" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B62" s="27" t="s">
+      <c r="B62" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="8">
-        <v>0</v>
-      </c>
-      <c r="D62" s="9">
-        <v>0</v>
-      </c>
-      <c r="E62" s="9">
+      <c r="C62" s="7">
+        <v>0</v>
+      </c>
+      <c r="D62" s="8">
+        <v>0</v>
+      </c>
+      <c r="E62" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F62" s="40"/>
-      <c r="H62" s="8">
-        <v>0</v>
-      </c>
-      <c r="I62" s="9">
-        <v>1</v>
-      </c>
-      <c r="J62" s="9">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K62" s="10"/>
-      <c r="M62" s="8">
-        <v>0</v>
-      </c>
-      <c r="N62" s="9">
-        <v>0</v>
-      </c>
-      <c r="O62" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P62" s="10"/>
-      <c r="Q62" s="12"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P63" s="1" t="s">
+      <c r="H62" s="7">
+        <v>0</v>
+      </c>
+      <c r="I62" s="8">
+        <v>1</v>
+      </c>
+      <c r="J62" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K62" s="36"/>
+      <c r="M62" s="7">
+        <v>0</v>
+      </c>
+      <c r="N62" s="8">
+        <v>1</v>
+      </c>
+      <c r="O62" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P62" s="44"/>
+      <c r="R62" s="7">
+        <v>0</v>
+      </c>
+      <c r="S62" s="8">
+        <v>0</v>
+      </c>
+      <c r="T62" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U62" s="36"/>
+      <c r="V62" s="32"/>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="U63" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q63">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P64" s="1" t="s">
+      <c r="V63">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="U64" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q64">
+      <c r="V64">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="16:17" x14ac:dyDescent="0.3">
-      <c r="P65" s="1" t="s">
+    <row r="65" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U65" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q65">
-        <v>5</v>
+      <c r="V65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="21:22" x14ac:dyDescent="0.3">
+      <c r="U66" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V66">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="84">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="Q45:Q47"/>
-    <mergeCell ref="Q48:Q50"/>
-    <mergeCell ref="Q51:Q53"/>
-    <mergeCell ref="Q54:Q56"/>
-    <mergeCell ref="Q57:Q59"/>
-    <mergeCell ref="Q60:Q62"/>
-    <mergeCell ref="Q27:Q29"/>
-    <mergeCell ref="Q30:Q32"/>
-    <mergeCell ref="Q33:Q35"/>
-    <mergeCell ref="Q36:Q38"/>
-    <mergeCell ref="Q39:Q41"/>
-    <mergeCell ref="Q42:Q44"/>
-    <mergeCell ref="P57:P59"/>
+  <mergeCells count="105">
     <mergeCell ref="P60:P62"/>
-    <mergeCell ref="Q3:Q5"/>
-    <mergeCell ref="Q6:Q8"/>
-    <mergeCell ref="Q9:Q11"/>
-    <mergeCell ref="Q12:Q14"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="Q18:Q20"/>
-    <mergeCell ref="Q21:Q23"/>
-    <mergeCell ref="Q24:Q26"/>
-    <mergeCell ref="P39:P41"/>
-    <mergeCell ref="P42:P44"/>
     <mergeCell ref="P45:P47"/>
     <mergeCell ref="P48:P50"/>
     <mergeCell ref="P51:P53"/>
     <mergeCell ref="P54:P56"/>
+    <mergeCell ref="P57:P59"/>
+    <mergeCell ref="P30:P32"/>
+    <mergeCell ref="P33:P35"/>
+    <mergeCell ref="P36:P38"/>
+    <mergeCell ref="P39:P41"/>
+    <mergeCell ref="P42:P44"/>
+    <mergeCell ref="P15:P17"/>
+    <mergeCell ref="P18:P20"/>
     <mergeCell ref="P21:P23"/>
     <mergeCell ref="P24:P26"/>
     <mergeCell ref="P27:P29"/>
-    <mergeCell ref="P30:P32"/>
-    <mergeCell ref="P33:P35"/>
-    <mergeCell ref="P36:P38"/>
+    <mergeCell ref="M1:P1"/>
     <mergeCell ref="P3:P5"/>
     <mergeCell ref="P6:P8"/>
     <mergeCell ref="P9:P11"/>
     <mergeCell ref="P12:P14"/>
-    <mergeCell ref="P15:P17"/>
-    <mergeCell ref="P18:P20"/>
-    <mergeCell ref="K45:K47"/>
-    <mergeCell ref="K48:K50"/>
-    <mergeCell ref="K51:K53"/>
-    <mergeCell ref="K54:K56"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K27:K29"/>
-    <mergeCell ref="K30:K32"/>
-    <mergeCell ref="K33:K35"/>
-    <mergeCell ref="K36:K38"/>
-    <mergeCell ref="K39:K41"/>
-    <mergeCell ref="K42:K44"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="F33:F35"/>
     <mergeCell ref="F57:F59"/>
     <mergeCell ref="F60:F62"/>
     <mergeCell ref="K3:K5"/>
@@ -4284,18 +5047,62 @@
     <mergeCell ref="F48:F50"/>
     <mergeCell ref="F51:F53"/>
     <mergeCell ref="F54:F56"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K27:K29"/>
+    <mergeCell ref="K30:K32"/>
+    <mergeCell ref="K33:K35"/>
+    <mergeCell ref="K36:K38"/>
+    <mergeCell ref="K39:K41"/>
+    <mergeCell ref="K42:K44"/>
+    <mergeCell ref="K45:K47"/>
+    <mergeCell ref="K48:K50"/>
+    <mergeCell ref="K51:K53"/>
+    <mergeCell ref="K54:K56"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="U36:U38"/>
+    <mergeCell ref="U3:U5"/>
+    <mergeCell ref="U6:U8"/>
+    <mergeCell ref="U9:U11"/>
+    <mergeCell ref="U12:U14"/>
+    <mergeCell ref="U15:U17"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="U57:U59"/>
+    <mergeCell ref="U60:U62"/>
+    <mergeCell ref="V3:V5"/>
+    <mergeCell ref="V6:V8"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="V12:V14"/>
+    <mergeCell ref="V15:V17"/>
+    <mergeCell ref="V18:V20"/>
+    <mergeCell ref="V21:V23"/>
+    <mergeCell ref="V24:V26"/>
+    <mergeCell ref="U39:U41"/>
+    <mergeCell ref="U42:U44"/>
+    <mergeCell ref="U45:U47"/>
+    <mergeCell ref="U48:U50"/>
+    <mergeCell ref="U51:U53"/>
+    <mergeCell ref="U54:U56"/>
+    <mergeCell ref="V48:V50"/>
+    <mergeCell ref="V51:V53"/>
+    <mergeCell ref="V54:V56"/>
+    <mergeCell ref="V57:V59"/>
+    <mergeCell ref="V60:V62"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="V45:V47"/>
+    <mergeCell ref="V27:V29"/>
+    <mergeCell ref="V30:V32"/>
+    <mergeCell ref="V33:V35"/>
+    <mergeCell ref="V36:V38"/>
+    <mergeCell ref="V39:V41"/>
+    <mergeCell ref="V42:V44"/>
+    <mergeCell ref="U21:U23"/>
+    <mergeCell ref="U24:U26"/>
+    <mergeCell ref="U27:U29"/>
+    <mergeCell ref="U30:U32"/>
+    <mergeCell ref="U33:U35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>